<commit_message>
assigmnt next week and SQL DB
</commit_message>
<xml_diff>
--- a/Assigment.xlsx
+++ b/Assigment.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -83,6 +83,21 @@
   </si>
   <si>
     <t>Chuyển đổi sang file aspx của màn hình  4/</t>
+  </si>
+  <si>
+    <t>Tuần 3</t>
+  </si>
+  <si>
+    <t>Validate các màn hình 4/</t>
+  </si>
+  <si>
+    <t>Validate các màn hình 2/ + 5/</t>
+  </si>
+  <si>
+    <t>Validate các màn hình 1/ + 3/</t>
+  </si>
+  <si>
+    <t>Thứ 4, 10/4/2019</t>
   </si>
 </sst>
 </file>
@@ -105,7 +120,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,6 +145,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -223,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -244,6 +265,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E23"/>
+  <dimension ref="A2:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -566,9 +588,10 @@
     <col min="3" max="3" width="22.875" customWidth="1"/>
     <col min="4" max="4" width="36.75" customWidth="1"/>
     <col min="5" max="5" width="40.375" customWidth="1"/>
+    <col min="6" max="6" width="19.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -580,8 +603,11 @@
       <c r="E2" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -594,8 +620,11 @@
       <c r="E3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -606,8 +635,11 @@
       <c r="E4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -618,8 +650,11 @@
       <c r="E5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -629,14 +664,17 @@
       <c r="D6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="16" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C10" s="9"/>
     </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>12</v>
       </c>
@@ -646,14 +684,14 @@
       <c r="C11" s="4"/>
       <c r="D11" s="11"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="12"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="4" t="s">
         <v>15</v>
@@ -661,7 +699,7 @@
       <c r="C13" s="4"/>
       <c r="D13" s="11"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="4" t="s">
         <v>16</v>
@@ -669,7 +707,7 @@
       <c r="C14" s="4"/>
       <c r="D14" s="11"/>
     </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="9" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
complete task week4 : Thach : Login
</commit_message>
<xml_diff>
--- a/Assigment.xlsx
+++ b/Assigment.xlsx
@@ -286,12 +286,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -302,6 +296,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,10 +633,10 @@
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="7"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="2" t="s">
         <v>18</v>
       </c>
@@ -651,7 +651,7 @@
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
@@ -671,7 +671,7 @@
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="16"/>
       <c r="D4" t="s">
         <v>8</v>
       </c>
@@ -689,7 +689,7 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="16"/>
       <c r="D5" t="s">
         <v>7</v>
       </c>
@@ -719,7 +719,7 @@
       <c r="F6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="15" t="s">
         <v>38</v>
       </c>
     </row>
@@ -730,79 +730,79 @@
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="8"/>
+      <c r="C11" s="6"/>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="B12" s="8" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="6"/>
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="B13" s="8" t="s">
+      <c r="A13" s="7"/>
+      <c r="B13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="8"/>
+      <c r="C13" s="6"/>
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="B14" s="8" t="s">
+      <c r="A14" s="7"/>
+      <c r="B14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="8"/>
+      <c r="C14" s="6"/>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8" t="s">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="8"/>
+      <c r="C15" s="6"/>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="10"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
-      <c r="B18" s="14" t="s">
+      <c r="A18" s="10"/>
+      <c r="B18" s="12" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="12"/>
-      <c r="B19" s="14" t="s">
+      <c r="A19" s="10"/>
+      <c r="B19" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="15"/>
-      <c r="B20" s="16" t="s">
+      <c r="A20" s="13"/>
+      <c r="B20" s="14" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>